<commit_message>
user so vota uma vez, vota em branco e nulo, limpeza de prints e bug fixes
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gui\Desktop\SD\Projeto-SD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E1BA05-3E4F-4DD4-BDB5-39BD82218DE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F155D8F7-51D6-451F-BA0E-B02EDFB14C3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10155" yWindow="3915" windowWidth="25605" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Requisitos Funcionais</t>
   </si>
@@ -235,9 +235,6 @@
   </si>
   <si>
     <t>ta sempre 60s e não atualiza</t>
-  </si>
-  <si>
-    <t>não permitir votar outra vez</t>
   </si>
 </sst>
 </file>
@@ -1039,10 +1036,10 @@
   <dimension ref="A1:D85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D47" sqref="D47"/>
+      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1054,13 +1051,13 @@
     <col min="5" max="16384" width="27.125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="2.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:4" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="2.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:3" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1068,7 +1065,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1076,7 +1073,7 @@
         <v>2017987654</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <f>A6+A21+A28+A35</f>
         <v>100</v>
@@ -1089,7 +1086,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <f>SUM(A7:A20)</f>
         <v>44</v>
@@ -1102,7 +1099,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -1113,7 +1110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>3</v>
       </c>
@@ -1124,7 +1121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>3</v>
       </c>
@@ -1135,7 +1132,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>3</v>
       </c>
@@ -1146,7 +1143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>3</v>
       </c>
@@ -1157,7 +1154,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>3</v>
       </c>
@@ -1168,7 +1165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>3</v>
       </c>
@@ -1179,21 +1176,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>3</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="13">
-        <v>3</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C14" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>3</v>
       </c>
@@ -1204,7 +1198,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>3</v>
       </c>
@@ -1279,7 +1273,7 @@
       <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="12">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
votos bem e udp finalmente bem!!!!!
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gui\Desktop\SD\Projeto-SD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370488DF-CED0-48B9-8978-EEFAA152A29D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747ED7C8-EECB-4B0E-9EBA-D365173881C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4845" yWindow="2430" windowWidth="25800" windowHeight="15615" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Requisitos Funcionais</t>
   </si>
@@ -238,9 +238,6 @@
   </si>
   <si>
     <t>Enunciado</t>
-  </si>
-  <si>
-    <t>Falta nr total de votos e percentagens</t>
   </si>
   <si>
     <t>Falta atualizar nr de eleitores que votaram em cada mesa</t>
@@ -325,7 +322,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -356,6 +353,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -523,7 +526,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -571,6 +574,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1072,10 +1078,10 @@
   <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1193,7 +1199,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" s="5">
         <v>4</v>
@@ -1282,7 +1288,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E16" s="5">
         <v>10</v>
@@ -1313,7 +1319,7 @@
         <v>3</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E18" s="5">
         <v>12</v>
@@ -1340,11 +1346,8 @@
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="13">
-        <v>3</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>59</v>
+      <c r="C20" s="12">
+        <v>3</v>
       </c>
       <c r="E20" s="16">
         <v>14</v>
@@ -1428,7 +1431,7 @@
       <c r="B27" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="19">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
locais de voto e bu fixes
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gui\Desktop\SD\Projeto-SD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747ED7C8-EECB-4B0E-9EBA-D365173881C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7601704-1C4F-4E10-84A8-BAB7E5EB2AA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4845" yWindow="2430" windowWidth="25800" windowHeight="15615" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4275" yWindow="2205" windowWidth="25800" windowHeight="15615" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2016-2017" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Requisitos Funcionais</t>
   </si>
@@ -240,13 +240,10 @@
     <t>Enunciado</t>
   </si>
   <si>
-    <t>Falta atualizar nr de eleitores que votaram em cada mesa</t>
-  </si>
-  <si>
-    <t>Em que mesa de voto e momento</t>
-  </si>
-  <si>
     <t>So pode haver uma mesa de Voto por departamento</t>
+  </si>
+  <si>
+    <t>momento</t>
   </si>
 </sst>
 </file>
@@ -1078,10 +1075,10 @@
   <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1199,7 +1196,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E10" s="5">
         <v>4</v>
@@ -1315,12 +1312,10 @@
       <c r="B18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="13">
-        <v>3</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>59</v>
-      </c>
+      <c r="C18" s="12">
+        <v>3</v>
+      </c>
+      <c r="D18" s="18"/>
       <c r="E18" s="5">
         <v>12</v>
       </c>
@@ -1466,7 +1461,7 @@
       <c r="B30" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="12">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
user esta a votar, udp bem e mais cenas
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gui\Desktop\SD\Projeto-SD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7601704-1C4F-4E10-84A8-BAB7E5EB2AA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9F3FD8-1BA8-4AD6-BEF9-DFC461F11100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="2205" windowWidth="25800" windowHeight="15615" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2016-2017" sheetId="2" r:id="rId1"/>
@@ -243,7 +243,7 @@
     <t>So pode haver uma mesa de Voto por departamento</t>
   </si>
   <si>
-    <t>momento</t>
+    <t>verificar se user esta a votar</t>
   </si>
 </sst>
 </file>
@@ -1078,7 +1078,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1178,7 +1178,7 @@
       <c r="B9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="13">
         <v>3</v>
       </c>
       <c r="E9" s="5">
@@ -1254,7 +1254,9 @@
       <c r="C14" s="12">
         <v>3</v>
       </c>
-      <c r="D14" s="18"/>
+      <c r="D14" s="18" t="s">
+        <v>60</v>
+      </c>
       <c r="E14" s="5">
         <v>8</v>
       </c>
@@ -1281,12 +1283,10 @@
       <c r="B16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="13">
-        <v>3</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>60</v>
-      </c>
+      <c r="C16" s="12">
+        <v>3</v>
+      </c>
+      <c r="D16" s="18"/>
       <c r="E16" s="5">
         <v>10</v>
       </c>
@@ -1494,7 +1494,7 @@
       <c r="B33" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="16">
+      <c r="C33" s="12">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
estado mesas de voto e terminais on/off
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gui\Desktop\SD\Projeto-SD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC4FC2D-D402-4873-B5C4-6C3D877DD99E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D64ACB1-75AF-4A2E-B817-89E810345581}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="2205" windowWidth="25800" windowHeight="15615" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-70" yWindow="15630" windowWidth="25800" windowHeight="15620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2016-2017" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Requisitos Funcionais</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>So pode haver uma mesa de Voto por departamento</t>
+  </si>
+  <si>
+    <t>On it</t>
   </si>
 </sst>
 </file>
@@ -520,7 +523,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -571,6 +574,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1075,7 +1081,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1178,6 +1184,9 @@
       <c r="C9" s="13">
         <v>3</v>
       </c>
+      <c r="D9" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="E9" s="5">
         <v>3</v>
       </c>
@@ -1189,7 +1198,7 @@
       <c r="B10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="13">
         <v>3</v>
       </c>
       <c r="D10" s="18" t="s">
@@ -1293,7 +1302,7 @@
       <c r="B17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="12">
         <v>3</v>
       </c>
       <c r="E17" s="5">
@@ -1374,7 +1383,7 @@
       <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="12">
         <v>4</v>
       </c>
     </row>
@@ -1385,7 +1394,7 @@
       <c r="B24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="19">
         <v>4</v>
       </c>
     </row>
@@ -1396,7 +1405,7 @@
       <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="20">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ultimas modificacoes contatempo e server
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gui\Desktop\SD\Projeto-SD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4092282cee5bc19f/Ambiente de Trabalho/UC/3ºano - 2º semestre/SD/Projeto-SD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0818C28F-E1C9-442D-8A92-79A20C39503C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0818C28F-E1C9-442D-8A92-79A20C39503C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="14290" windowWidth="25820" windowHeight="15620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2016-2017" sheetId="2" r:id="rId1"/>
@@ -1075,27 +1075,27 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B51" sqref="B51"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="27.09765625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.5" style="5" customWidth="1"/>
-    <col min="2" max="2" width="66.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="27.125" style="5"/>
-    <col min="4" max="4" width="58.625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="27.125" style="5"/>
-    <col min="6" max="6" width="52.125" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="27.125" style="5"/>
+    <col min="2" max="2" width="66.3984375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.09765625" style="5"/>
+    <col min="4" max="4" width="58.59765625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="27.09765625" style="5"/>
+    <col min="6" max="6" width="52.09765625" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="27.09765625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="2.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:5" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="2.1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:5" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>2017987654</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <f>A6+A21+A28+A35</f>
         <v>100</v>
@@ -1124,7 +1124,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <f>SUM(A7:A20)</f>
         <v>44</v>
@@ -1140,7 +1140,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>3</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>3</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>3</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>3</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>3</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>3</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>3</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>3</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>3</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>3</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>3</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>7</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>3</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <f>SUM(A22:A27)</f>
         <v>24</v>
@@ -1354,7 +1354,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>4</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>4</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>4</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>4</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="10">
         <v>4</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="10">
         <v>4</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <f>SUM(A29:A34)</f>
         <v>24</v>
@@ -1436,7 +1436,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>4</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>4</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>4</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="10">
         <v>4</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>4</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>4</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <f>SUM(A36:A39)</f>
         <v>8</v>
@@ -1515,7 +1515,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>2</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>2</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>2</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="10">
         <v>2</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B40" s="1" t="s">
         <v>8</v>
       </c>
@@ -1568,27 +1568,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B41" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B42" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B43" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B44" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B45" s="1" t="s">
         <v>9</v>
       </c>
@@ -1597,13 +1597,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B46" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C46" s="14"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B47" s="2" t="s">
         <v>13</v>
       </c>
@@ -1612,118 +1612,118 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B48" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C48" s="12"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B49" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C49" s="12"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B50" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C50" s="12"/>
     </row>
-    <row r="51" spans="2:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B51" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B52" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B53" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B54" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B55" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B56" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57" s="7"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B58" s="7"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B59" s="7"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B60" s="7"/>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B61" s="7"/>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B63" s="8"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B66" s="8"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B67" s="8"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B68" s="8"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B69" s="8"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B70" s="8"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B71" s="8"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B72" s="8"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B73" s="8"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B74" s="8"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B75" s="8"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B80" s="9"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B81" s="9"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B82" s="9"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B83" s="9"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B84" s="9"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B85" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
inicio do front end
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gui\Desktop\SD\Projeto-SD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02659ED-0855-44ED-9825-5DAECB6A7DF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16FB12C-3744-4DB4-8A07-6A318D500A03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="14290" windowWidth="25820" windowHeight="15620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="14180" windowWidth="25600" windowHeight="15620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2016-2017" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Requisitos Funcionais</t>
   </si>
@@ -229,12 +229,6 @@
   </si>
   <si>
     <t>Trazem duas máquinas (e.g., dois portáteis ou um portátil com uma VM)</t>
-  </si>
-  <si>
-    <t>RMI done; Falta multicast</t>
-  </si>
-  <si>
-    <t>ta sempre 60s e não atualiza</t>
   </si>
   <si>
     <t>Enunciado</t>
@@ -313,7 +307,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,12 +323,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -517,7 +505,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -549,28 +537,25 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1072,10 +1057,10 @@
   <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B54" sqref="B54"/>
+      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1137,7 +1122,7 @@
         <v>44</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1192,7 +1177,7 @@
       <c r="C10" s="12">
         <v>3</v>
       </c>
-      <c r="D10" s="18"/>
+      <c r="D10" s="16"/>
       <c r="E10" s="5">
         <v>4</v>
       </c>
@@ -1249,7 +1234,7 @@
       <c r="C14" s="12">
         <v>3</v>
       </c>
-      <c r="D14" s="18"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="5">
         <v>8</v>
       </c>
@@ -1264,7 +1249,7 @@
       <c r="C15" s="12">
         <v>3</v>
       </c>
-      <c r="D15" s="18"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="5">
         <v>9</v>
       </c>
@@ -1279,7 +1264,7 @@
       <c r="C16" s="12">
         <v>3</v>
       </c>
-      <c r="D16" s="18"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="5">
         <v>10</v>
       </c>
@@ -1308,7 +1293,7 @@
       <c r="C18" s="12">
         <v>3</v>
       </c>
-      <c r="D18" s="18"/>
+      <c r="D18" s="16"/>
       <c r="E18" s="5">
         <v>12</v>
       </c>
@@ -1323,7 +1308,7 @@
       <c r="C19" s="12">
         <v>7</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="15">
         <v>13</v>
       </c>
     </row>
@@ -1337,7 +1322,7 @@
       <c r="C20" s="12">
         <v>3</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="14">
         <v>14</v>
       </c>
     </row>
@@ -1383,7 +1368,7 @@
       <c r="B24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="17">
         <v>4</v>
       </c>
     </row>
@@ -1394,7 +1379,7 @@
       <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="20">
+      <c r="C25" s="18">
         <v>4</v>
       </c>
     </row>
@@ -1405,11 +1390,8 @@
       <c r="B26" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="15">
-        <v>4</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>57</v>
+      <c r="C26" s="19">
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1419,7 +1401,7 @@
       <c r="B27" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="19">
+      <c r="C27" s="17">
         <v>4</v>
       </c>
     </row>
@@ -1480,7 +1462,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>4</v>
       </c>
@@ -1491,7 +1473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>4</v>
       </c>
@@ -1502,7 +1484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <f>SUM(A36:A39)</f>
         <v>8</v>
@@ -1515,7 +1497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>2</v>
       </c>
@@ -1526,7 +1508,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>2</v>
       </c>
@@ -1537,7 +1519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>2</v>
       </c>
@@ -1548,7 +1530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="10">
         <v>2</v>
       </c>
@@ -1559,7 +1541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
         <v>8</v>
       </c>
@@ -1568,27 +1550,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
         <v>9</v>
       </c>
@@ -1597,22 +1579,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C46" s="14"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C46" s="13"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C47" s="13"/>
-      <c r="D47" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C47" s="12"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
         <v>49</v>
       </c>

</xml_diff>